<commit_message>
Added 10% features to acceptance test plan
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan (1).xlsx
+++ b/etc/Acceptance Test Plan (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacks\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klest\vs_proj\team-project-2225-swen-261-01-6f-we_bought_a_zoo\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CF5104-F9EC-49EA-AE87-EA684AB8F689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF32E1C-B473-488B-A051-815D53AA57B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="241" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="241" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>Instructions</t>
   </si>
@@ -105,15 +105,9 @@
     <t>Given a product is not in the inventory when I input a product object to be added then the product should be added to the inventory and be viewable on the catalog</t>
   </si>
   <si>
-    <t>Given a product is in the inventory when I input a product object to be added then the product's stock should increase by one</t>
-  </si>
-  <si>
     <t>As an owner I want to remove products from the catalog so that it can be up to date with the on hand inventory.</t>
   </si>
   <si>
-    <t>Given a product exists in the inventory when I remove the object then it should no longer be in the inventory and should not be viewable in the catalog.</t>
-  </si>
-  <si>
     <t>Given multiple of a product is in the inventory when I remove the product then the product's stock should decrease by one.</t>
   </si>
   <si>
@@ -123,15 +117,9 @@
     <t>Given a product exists in the inventory when I input another product to update then it should change that product to match the new product.</t>
   </si>
   <si>
-    <t>As a owner I want to be able to view customer info such as name, email address, and contact information so that I can keep track of my users.</t>
-  </si>
-  <si>
     <t>Given a user exists when I input the user ID then it should return the customer object associated with that user.</t>
   </si>
   <si>
-    <t>As a owner I want to be able to view customer billing information so that I can complete invoices for rentals.</t>
-  </si>
-  <si>
     <t>Given a customer exists when I input a user ID then it should return the customer's billing information.</t>
   </si>
   <si>
@@ -157,13 +145,64 @@
   </si>
   <si>
     <t>KL; 3/20/23; Backend for this worked but a bean error has popped up that we cant fix and therefore we cant run our application.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>As an owner I want to be able to view customer billing information so that I can complete invoices for rentals.</t>
+  </si>
+  <si>
+    <t>As an owner I want to be able to view customer info such as name, email address, and contact information so that I can keep track of my users.</t>
+  </si>
+  <si>
+    <t>Given a species exists when I input new information for that species then it should add a new information piece for that species.</t>
+  </si>
+  <si>
+    <t>Given a species does not exist when I input new information for that species then it will not add any information.</t>
+  </si>
+  <si>
+    <t>Given a piece of information exists when press remove on that information piece then it should remove that piece of information.</t>
+  </si>
+  <si>
+    <t>As an owner I want to add and remove information so that I can keep the care information up to date.</t>
+  </si>
+  <si>
+    <t>As an owner I want to be able to update information so that I can make sure all information is accuate and am able to change it as I see fit</t>
+  </si>
+  <si>
+    <t>Given an information piece exists when I input an update to that information then the information should be replaced with what I input to update it.</t>
+  </si>
+  <si>
+    <t>As a customer I want to be able to browse species information so that I can see how to take care of all species before I purchase one.</t>
+  </si>
+  <si>
+    <t>Given information exists when I log in as a user then I should be able to navigate to, and view all species care information.</t>
+  </si>
+  <si>
+    <t>As a customer I want to receive information for the animals I have purchased so that I can quickly find information on the animals I have rented.</t>
+  </si>
+  <si>
+    <t>Given that I check out with my products, when I finalize my purchase, then I want to receive comprehensive information on how to care for those specific animals</t>
+  </si>
+  <si>
+    <t>10% Feature, not worked on in this sprint</t>
+  </si>
+  <si>
+    <t>4/1/2023 Not being implemented during this project</t>
+  </si>
+  <si>
+    <t>Team; 4/1/2023 Not being implemented during this project</t>
+  </si>
+  <si>
+    <t>KL; 4/1/2023; Users cannot change their information after being registered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,6 +223,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -198,6 +238,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF172B4D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF172B4D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF172B4D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +272,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -244,11 +309,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -284,11 +437,185 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -706,11 +1033,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F587"/>
+  <dimension ref="A1:F585"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -746,34 +1073,40 @@
     </row>
     <row r="2" spans="1:6" ht="42" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="E4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -783,12 +1116,14 @@
         <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
@@ -796,7 +1131,9 @@
         <v>15</v>
       </c>
       <c r="C6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
@@ -806,12 +1143,14 @@
         <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -821,12 +1160,14 @@
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
@@ -834,7 +1175,12 @@
         <v>19</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -844,12 +1190,14 @@
         <v>21</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
@@ -857,7 +1205,9 @@
         <v>22</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -867,334 +1217,432 @@
         <v>23</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="62" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="93" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="31" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" ht="62" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="8"/>
+      <c r="B15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" ht="93" x14ac:dyDescent="0.35">
+      <c r="F15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="F16" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="8"/>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" ht="62" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>34</v>
-      </c>
+    <row r="18" spans="1:5" ht="31" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="8"/>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A19" s="18"/>
+      <c r="B19" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="C19" s="8"/>
+      <c r="D19" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="C20" s="8"/>
+      <c r="D20" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>48</v>
+      </c>
       <c r="C21" s="8"/>
+      <c r="D21" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>50</v>
+      </c>
       <c r="C22" s="8"/>
+      <c r="D22" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="19"/>
       <c r="C23" s="8"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="19"/>
       <c r="C24" s="8"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="19"/>
       <c r="C25" s="8"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="19"/>
       <c r="C26" s="8"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="19"/>
       <c r="C27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="19"/>
       <c r="C28" s="8"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="19"/>
       <c r="C29" s="8"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="19"/>
       <c r="C30" s="8"/>
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="19"/>
       <c r="C31" s="8"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="19"/>
       <c r="C32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="19"/>
       <c r="C33" s="8"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="19"/>
       <c r="C34" s="8"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="19"/>
       <c r="C35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="19"/>
       <c r="C36" s="8"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="19"/>
       <c r="C37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="19"/>
       <c r="C38" s="8"/>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="19"/>
       <c r="C39" s="8"/>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="19"/>
       <c r="C40" s="8"/>
       <c r="E40" s="8"/>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="19"/>
       <c r="C41" s="8"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="19"/>
       <c r="C42" s="8"/>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="19"/>
       <c r="C43" s="8"/>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="19"/>
       <c r="C44" s="8"/>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="19"/>
       <c r="C45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="19"/>
       <c r="C46" s="8"/>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="19"/>
       <c r="C47" s="8"/>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="19"/>
       <c r="C48" s="8"/>
       <c r="E48" s="8"/>
     </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="19"/>
       <c r="C49" s="8"/>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="19"/>
       <c r="C50" s="8"/>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="19"/>
       <c r="C51" s="8"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="19"/>
       <c r="C52" s="8"/>
       <c r="E52" s="8"/>
     </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="19"/>
       <c r="C53" s="8"/>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="19"/>
       <c r="C54" s="8"/>
       <c r="E54" s="8"/>
     </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="19"/>
       <c r="C55" s="8"/>
       <c r="E55" s="8"/>
     </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="19"/>
       <c r="C56" s="8"/>
       <c r="E56" s="8"/>
     </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="19"/>
       <c r="C57" s="8"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="19"/>
       <c r="C58" s="8"/>
       <c r="E58" s="8"/>
     </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="19"/>
       <c r="C59" s="8"/>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="19"/>
       <c r="C60" s="8"/>
       <c r="E60" s="8"/>
     </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="19"/>
       <c r="C61" s="8"/>
       <c r="E61" s="8"/>
     </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="19"/>
       <c r="C62" s="8"/>
       <c r="E62" s="8"/>
     </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="19"/>
       <c r="C63" s="8"/>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="19"/>
       <c r="C64" s="8"/>
       <c r="E64" s="8"/>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="19"/>
       <c r="C65" s="8"/>
       <c r="E65" s="8"/>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="19"/>
       <c r="C66" s="8"/>
       <c r="E66" s="8"/>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C67" s="8"/>
       <c r="E67" s="8"/>
     </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C68" s="8"/>
       <c r="E68" s="8"/>
     </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C69" s="8"/>
       <c r="E69" s="8"/>
     </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C70" s="8"/>
       <c r="E70" s="8"/>
     </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C71" s="8"/>
       <c r="E71" s="8"/>
     </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C72" s="8"/>
       <c r="E72" s="8"/>
     </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C73" s="8"/>
       <c r="E73" s="8"/>
     </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C74" s="8"/>
       <c r="E74" s="8"/>
     </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C75" s="8"/>
       <c r="E75" s="8"/>
     </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C76" s="8"/>
       <c r="E76" s="8"/>
     </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C77" s="8"/>
       <c r="E77" s="8"/>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C78" s="8"/>
       <c r="E78" s="8"/>
     </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C79" s="8"/>
       <c r="E79" s="8"/>
     </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C80" s="8"/>
       <c r="E80" s="8"/>
     </row>
@@ -3218,34 +3666,34 @@
       <c r="C585" s="8"/>
       <c r="E585" s="8"/>
     </row>
-    <row r="586" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C586" s="8"/>
-      <c r="E586" s="8"/>
-    </row>
-    <row r="587" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C587" s="8"/>
-      <c r="E587" s="8"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C2:C587 E2:E587">
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
+  <conditionalFormatting sqref="C2:C585 E2:E585">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>"Not Implemented"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D587 F2:F587">
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="D2:D585 F2:F585">
+    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"Not Implemented"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C587 E2:E587" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C585 E2:E585" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>